<commit_message>
Dialing in on figuring out how to make slow animation movement look right
</commit_message>
<xml_diff>
--- a/animations/f_slow_stop.xlsx
+++ b/animations/f_slow_stop.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B347288-8E30-3F42-804C-529A3DD9EB6E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F710562A-9193-8C48-9D3B-0E0C7FDECC4D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="50200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="50260" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -131,7 +127,56 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -430,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW44"/>
+  <dimension ref="A1:AW81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="266" zoomScaleNormal="266" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="266" zoomScaleNormal="266" workbookViewId="0">
+      <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -472,37 +517,28 @@
         <v>9</v>
       </c>
       <c r="J1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q1">
-        <v>8</v>
-      </c>
-      <c r="R1">
-        <v>9</v>
-      </c>
-      <c r="S1">
-        <v>1</v>
-      </c>
-      <c r="T1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="U1"/>
     </row>
@@ -536,23 +572,26 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I3">
         <v>7</v>
@@ -562,20 +601,23 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>1</v>
+      </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4">
         <v>6</v>
@@ -588,17 +630,20 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I5">
         <v>5</v>
@@ -611,14 +656,17 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>1</v>
+      </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -627,18 +675,21 @@
         <v>5</v>
       </c>
       <c r="K6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L6">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>1</v>
+      </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I7">
         <v>3</v>
@@ -647,15 +698,18 @@
         <v>4</v>
       </c>
       <c r="K7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L7">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>1</v>
+      </c>
       <c r="H8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -664,13 +718,16 @@
         <v>3</v>
       </c>
       <c r="K8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L8">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>1</v>
+      </c>
       <c r="I9">
         <v>1</v>
       </c>
@@ -678,10 +735,10 @@
         <v>2</v>
       </c>
       <c r="K9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M9">
         <v>8</v>
@@ -692,10 +749,10 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M10">
         <v>8</v>
@@ -703,18 +760,21 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="K11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M11">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>1</v>
+      </c>
       <c r="L12">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M12">
         <v>8</v>
@@ -722,316 +782,941 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L13">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M13">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <v>1</v>
+      </c>
       <c r="L14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M14">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>2</v>
+      </c>
       <c r="L15">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M15">
         <v>8</v>
       </c>
-      <c r="N15">
-        <v>8</v>
-      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>3</v>
+      </c>
       <c r="L16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M16">
         <v>8</v>
       </c>
-      <c r="N16">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <v>4</v>
+      </c>
       <c r="L17">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M17">
         <v>8</v>
       </c>
-      <c r="N17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <v>5</v>
+      </c>
       <c r="L18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M18">
         <v>8</v>
       </c>
-      <c r="N18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <v>6</v>
+      </c>
       <c r="L19">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M19">
-        <v>7</v>
-      </c>
-      <c r="N19">
-        <v>8</v>
-      </c>
-      <c r="O19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <v>7</v>
+      </c>
       <c r="L20">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M20">
-        <v>6</v>
-      </c>
-      <c r="N20">
-        <v>8</v>
-      </c>
-      <c r="O20">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <v>8</v>
+      </c>
       <c r="L21">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M21">
-        <v>5</v>
-      </c>
-      <c r="N21">
-        <v>8</v>
-      </c>
-      <c r="O21">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <v>8</v>
+      </c>
       <c r="L22">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M22">
-        <v>4</v>
-      </c>
-      <c r="N22">
-        <v>7</v>
-      </c>
-      <c r="O22">
-        <v>8</v>
-      </c>
-      <c r="P22">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <v>8</v>
+      </c>
       <c r="L23">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M23">
-        <v>3</v>
-      </c>
-      <c r="N23">
-        <v>6</v>
-      </c>
-      <c r="O23">
-        <v>8</v>
-      </c>
-      <c r="P23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>8</v>
+      </c>
       <c r="L24">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M24">
-        <v>2</v>
-      </c>
-      <c r="N24">
-        <v>5</v>
-      </c>
-      <c r="O24">
-        <v>7</v>
-      </c>
-      <c r="P24">
-        <v>8</v>
-      </c>
-      <c r="Q24">
-        <v>8</v>
-      </c>
-      <c r="U24"/>
-    </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>8</v>
+      </c>
       <c r="L25">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M25">
-        <v>2</v>
-      </c>
-      <c r="N25">
-        <v>4</v>
-      </c>
-      <c r="O25">
-        <v>6</v>
-      </c>
-      <c r="P25">
-        <v>7</v>
-      </c>
-      <c r="Q25">
-        <v>8</v>
-      </c>
-      <c r="R25">
-        <v>8</v>
-      </c>
-      <c r="U25"/>
-    </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="J26" s="5">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>8</v>
+      </c>
       <c r="L26">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="M26">
         <v>2</v>
       </c>
-      <c r="N26">
-        <v>3</v>
-      </c>
-      <c r="O26">
-        <v>5</v>
-      </c>
-      <c r="P26">
-        <v>6</v>
-      </c>
-      <c r="Q26">
-        <v>7</v>
-      </c>
-      <c r="R26">
-        <v>8</v>
-      </c>
-      <c r="S26">
-        <v>8</v>
-      </c>
-      <c r="U26"/>
-    </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27" s="6">
+        <v>3</v>
+      </c>
+      <c r="K27">
+        <v>8</v>
+      </c>
       <c r="L27">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M27">
-        <v>2</v>
-      </c>
-      <c r="N27">
-        <v>3</v>
-      </c>
-      <c r="O27">
-        <v>4</v>
-      </c>
-      <c r="P27">
-        <v>5</v>
-      </c>
-      <c r="Q27">
-        <v>6</v>
-      </c>
-      <c r="R27">
-        <v>7</v>
-      </c>
-      <c r="S27">
-        <v>8</v>
-      </c>
-      <c r="T27">
-        <v>8</v>
-      </c>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-    </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="AV31" s="2"/>
-    </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="AO32" s="2"/>
-      <c r="AP32" s="3"/>
-      <c r="AV32" s="2"/>
-      <c r="AW32" s="3"/>
-    </row>
-    <row r="33" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AO33" s="2"/>
-      <c r="AP33" s="3"/>
-      <c r="AV33" s="2"/>
-      <c r="AW33" s="3"/>
-    </row>
-    <row r="34" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AO34" s="2"/>
-      <c r="AP34" s="3"/>
-      <c r="AU34" s="2"/>
-      <c r="AV34" s="3"/>
-    </row>
-    <row r="35" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AO35" s="3"/>
-      <c r="AP35" s="2"/>
-      <c r="AU35" s="3"/>
-      <c r="AV35" s="2"/>
-    </row>
-    <row r="36" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AO36" s="3"/>
-      <c r="AP36" s="2"/>
-      <c r="AU36" s="3"/>
-    </row>
-    <row r="37" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AO37" s="3"/>
-      <c r="AP37" s="2"/>
-    </row>
-    <row r="38" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AO38" s="3"/>
-      <c r="AP38" s="2"/>
-    </row>
-    <row r="39" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AO39" s="3"/>
-      <c r="AP39" s="2"/>
-    </row>
-    <row r="40" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AP40" s="2"/>
-    </row>
-    <row r="41" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AP41" s="2"/>
-    </row>
-    <row r="42" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AP42" s="2"/>
-    </row>
-    <row r="43" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AP43" s="2"/>
-    </row>
-    <row r="44" spans="41:49" x14ac:dyDescent="0.2">
-      <c r="AP44" s="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28" s="7">
+        <v>4</v>
+      </c>
+      <c r="K28">
+        <v>8</v>
+      </c>
+      <c r="L28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="J29" s="8">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <v>8</v>
+      </c>
+      <c r="L29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I30">
+        <v>5</v>
+      </c>
+      <c r="J30" s="9">
+        <v>6</v>
+      </c>
+      <c r="K30">
+        <v>8</v>
+      </c>
+      <c r="L30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I31">
+        <v>6</v>
+      </c>
+      <c r="J31" s="10">
+        <v>7</v>
+      </c>
+      <c r="K31">
+        <v>8</v>
+      </c>
+      <c r="L31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I32">
+        <v>7</v>
+      </c>
+      <c r="J32">
+        <v>8</v>
+      </c>
+      <c r="K32">
+        <v>8</v>
+      </c>
+      <c r="L32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="I33">
+        <v>8</v>
+      </c>
+      <c r="J33">
+        <v>8</v>
+      </c>
+      <c r="K33">
+        <v>7</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="H34">
+        <v>5</v>
+      </c>
+      <c r="I34">
+        <v>8</v>
+      </c>
+      <c r="J34">
+        <v>7</v>
+      </c>
+      <c r="K34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="H35">
+        <v>6</v>
+      </c>
+      <c r="I35">
+        <v>8</v>
+      </c>
+      <c r="J35">
+        <v>6</v>
+      </c>
+      <c r="K35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="H36">
+        <v>7</v>
+      </c>
+      <c r="I36">
+        <v>8</v>
+      </c>
+      <c r="J36">
+        <v>5</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>8</v>
+      </c>
+      <c r="I37">
+        <v>8</v>
+      </c>
+      <c r="J37">
+        <v>4</v>
+      </c>
+      <c r="K37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38">
+        <v>8</v>
+      </c>
+      <c r="I38">
+        <v>8</v>
+      </c>
+      <c r="J38">
+        <v>3</v>
+      </c>
+      <c r="K38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>6</v>
+      </c>
+      <c r="H39">
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <v>8</v>
+      </c>
+      <c r="J39">
+        <v>2</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>7</v>
+      </c>
+      <c r="H40">
+        <v>8</v>
+      </c>
+      <c r="I40">
+        <v>8</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>5</v>
+      </c>
+      <c r="G41">
+        <v>8</v>
+      </c>
+      <c r="H41">
+        <v>8</v>
+      </c>
+      <c r="I41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>6</v>
+      </c>
+      <c r="G42">
+        <v>8</v>
+      </c>
+      <c r="H42">
+        <v>8</v>
+      </c>
+      <c r="I42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>7</v>
+      </c>
+      <c r="G43">
+        <v>8</v>
+      </c>
+      <c r="H43">
+        <v>7</v>
+      </c>
+      <c r="I43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>8</v>
+      </c>
+      <c r="G44">
+        <v>8</v>
+      </c>
+      <c r="H44">
+        <v>6</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>8</v>
+      </c>
+      <c r="G45">
+        <v>8</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+      <c r="I45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>7</v>
+      </c>
+      <c r="G46">
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <v>8</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>6</v>
+      </c>
+      <c r="G47">
+        <v>8</v>
+      </c>
+      <c r="H47">
+        <v>8</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>5</v>
+      </c>
+      <c r="G48">
+        <v>7</v>
+      </c>
+      <c r="H48">
+        <v>8</v>
+      </c>
+      <c r="I48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>4</v>
+      </c>
+      <c r="G49">
+        <v>6</v>
+      </c>
+      <c r="H49">
+        <v>7</v>
+      </c>
+      <c r="I49">
+        <v>8</v>
+      </c>
+      <c r="J49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50">
+        <v>6</v>
+      </c>
+      <c r="I50">
+        <v>7</v>
+      </c>
+      <c r="J50">
+        <v>8</v>
+      </c>
+      <c r="K50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51">
+        <v>4</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <v>6</v>
+      </c>
+      <c r="J51">
+        <v>8</v>
+      </c>
+      <c r="K51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="H52">
+        <v>4</v>
+      </c>
+      <c r="I52">
+        <v>5</v>
+      </c>
+      <c r="J52">
+        <v>8</v>
+      </c>
+      <c r="K52">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53">
+        <v>3</v>
+      </c>
+      <c r="I53">
+        <v>4</v>
+      </c>
+      <c r="J53">
+        <v>7</v>
+      </c>
+      <c r="K53">
+        <v>8</v>
+      </c>
+      <c r="L53">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54">
+        <v>3</v>
+      </c>
+      <c r="J54">
+        <v>6</v>
+      </c>
+      <c r="K54">
+        <v>8</v>
+      </c>
+      <c r="L54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+      <c r="J55">
+        <v>5</v>
+      </c>
+      <c r="K55">
+        <v>8</v>
+      </c>
+      <c r="L55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="H56">
+        <v>2</v>
+      </c>
+      <c r="I56">
+        <v>2</v>
+      </c>
+      <c r="J56">
+        <v>4</v>
+      </c>
+      <c r="K56">
+        <v>7</v>
+      </c>
+      <c r="L56">
+        <v>8</v>
+      </c>
+      <c r="M56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="10"/>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>2</v>
+      </c>
+      <c r="J57">
+        <v>3</v>
+      </c>
+      <c r="K57">
+        <v>6</v>
+      </c>
+      <c r="L57">
+        <v>8</v>
+      </c>
+      <c r="M57">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="I58">
+        <v>2</v>
+      </c>
+      <c r="J58">
+        <v>2</v>
+      </c>
+      <c r="K58">
+        <v>5</v>
+      </c>
+      <c r="L58">
+        <v>7</v>
+      </c>
+      <c r="M58">
+        <v>8</v>
+      </c>
+      <c r="N58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>2</v>
+      </c>
+      <c r="K59">
+        <v>4</v>
+      </c>
+      <c r="L59">
+        <v>6</v>
+      </c>
+      <c r="M59">
+        <v>7</v>
+      </c>
+      <c r="N59">
+        <v>8</v>
+      </c>
+      <c r="O59">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>2</v>
+      </c>
+      <c r="K60">
+        <v>3</v>
+      </c>
+      <c r="L60">
+        <v>5</v>
+      </c>
+      <c r="M60">
+        <v>6</v>
+      </c>
+      <c r="N60">
+        <v>7</v>
+      </c>
+      <c r="O60">
+        <v>8</v>
+      </c>
+      <c r="P60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>2</v>
+      </c>
+      <c r="K61">
+        <v>3</v>
+      </c>
+      <c r="L61">
+        <v>4</v>
+      </c>
+      <c r="M61">
+        <v>5</v>
+      </c>
+      <c r="N61">
+        <v>6</v>
+      </c>
+      <c r="O61">
+        <v>7</v>
+      </c>
+      <c r="P61">
+        <v>8</v>
+      </c>
+      <c r="Q61">
+        <v>8</v>
+      </c>
+      <c r="U61"/>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>2</v>
+      </c>
+      <c r="K62">
+        <v>3</v>
+      </c>
+      <c r="L62">
+        <v>5</v>
+      </c>
+      <c r="M62">
+        <v>6</v>
+      </c>
+      <c r="N62">
+        <v>7</v>
+      </c>
+      <c r="O62">
+        <v>8</v>
+      </c>
+      <c r="P62">
+        <v>8</v>
+      </c>
+      <c r="U62"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>2</v>
+      </c>
+      <c r="K63">
+        <v>3</v>
+      </c>
+      <c r="L63">
+        <v>4</v>
+      </c>
+      <c r="M63">
+        <v>5</v>
+      </c>
+      <c r="N63">
+        <v>6</v>
+      </c>
+      <c r="O63">
+        <v>7</v>
+      </c>
+      <c r="P63">
+        <v>8</v>
+      </c>
+      <c r="Q63">
+        <v>8</v>
+      </c>
+      <c r="U63"/>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>2</v>
+      </c>
+      <c r="K64">
+        <v>3</v>
+      </c>
+      <c r="L64">
+        <v>5</v>
+      </c>
+      <c r="M64">
+        <v>6</v>
+      </c>
+      <c r="N64">
+        <v>7</v>
+      </c>
+      <c r="O64">
+        <v>8</v>
+      </c>
+      <c r="P64">
+        <v>8</v>
+      </c>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+    </row>
+    <row r="65" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>2</v>
+      </c>
+      <c r="K65">
+        <v>3</v>
+      </c>
+      <c r="L65">
+        <v>4</v>
+      </c>
+      <c r="M65">
+        <v>5</v>
+      </c>
+      <c r="N65">
+        <v>6</v>
+      </c>
+      <c r="O65">
+        <v>7</v>
+      </c>
+      <c r="P65">
+        <v>8</v>
+      </c>
+      <c r="Q65">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AV68" s="2"/>
+    </row>
+    <row r="69" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AO69" s="2"/>
+      <c r="AP69" s="3"/>
+      <c r="AV69" s="2"/>
+      <c r="AW69" s="3"/>
+    </row>
+    <row r="70" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AO70" s="2"/>
+      <c r="AP70" s="3"/>
+      <c r="AV70" s="2"/>
+      <c r="AW70" s="3"/>
+    </row>
+    <row r="71" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AO71" s="2"/>
+      <c r="AP71" s="3"/>
+      <c r="AU71" s="2"/>
+      <c r="AV71" s="3"/>
+    </row>
+    <row r="72" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AO72" s="3"/>
+      <c r="AP72" s="2"/>
+      <c r="AU72" s="3"/>
+      <c r="AV72" s="2"/>
+    </row>
+    <row r="73" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AO73" s="3"/>
+      <c r="AP73" s="2"/>
+      <c r="AU73" s="3"/>
+    </row>
+    <row r="74" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AO74" s="3"/>
+      <c r="AP74" s="2"/>
+    </row>
+    <row r="75" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AO75" s="3"/>
+      <c r="AP75" s="2"/>
+    </row>
+    <row r="76" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AO76" s="3"/>
+      <c r="AP76" s="2"/>
+    </row>
+    <row r="77" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AP77" s="2"/>
+    </row>
+    <row r="78" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AP78" s="2"/>
+    </row>
+    <row r="79" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AP79" s="2"/>
+    </row>
+    <row r="80" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AP80" s="2"/>
+    </row>
+    <row r="81" spans="42:42" x14ac:dyDescent="0.2">
+      <c r="AP81" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H20:N20 AI29:AT29 AW34:BT81 AS29:XFD38 A34:AQ38 A29:AP33 AV30:AW39 AK30:BD30 AV34:BI59 AR30:BI38 AY30:BD44 AN31:AP39 AO31:AV31 A39:XFD1048576 AQ31:BH38 AU34:BH57 AT37:BB57 AQ31:BC44 AS38:BB57 A21:N21 O20:XFD21 N19:O21 A22:XFD28 A1:XFD19">
-    <cfRule type="containsBlanks" dxfId="1" priority="5">
+  <conditionalFormatting sqref="AI66:AT66 AW71:BT118 AS66:XFD75 A71:AQ75 A66:AP70 AV67:AW76 AK67:BD67 AV71:BI96 AR67:BI75 AY67:BD81 AN68:AP76 AO68:AV68 A76:XFD1048576 AQ68:BH75 AU71:BH94 AT74:BB94 AQ68:BC81 AS75:BB94 J57:XFD58 A58:N58 I58:Q59 A59:XFD65 H49:Q57 A26:I31 K26:XFD31 A21:XFD25 A14:J20 L14:XFD20 A1:XFD13 A32:XFD56 J49:Q63">
+    <cfRule type="containsBlanks" dxfId="8" priority="18">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1042,8 +1727,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:N20 A21:N21 O20:XFD21 N19:O21 A22:XFD1048576 A1:XFD19">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="J57:XFD58 A58:N58 I58:Q59 A59:XFD1048576 H49:Q57 A26:I31 K26:XFD31 A21:XFD25 A14:J20 L14:XFD20 A1:XFD13 A32:XFD56 J49:Q63">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="4"/>
@@ -1053,10 +1738,10 @@
         <color rgb="FFF5F0FF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
+    <cfRule type="containsBlanks" dxfId="7" priority="15">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1066,7 +1751,7 @@
         <color rgb="FFF5F0FF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="percentile" val="50"/>
@@ -1077,6 +1762,111 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="containsBlanks" dxfId="4" priority="12">
+      <formula>LEN(TRIM(K14))=0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF4B317F"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="4"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF331966"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="3" priority="9">
+      <formula>LEN(TRIM(K14))=0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF4B317F"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF4B317F"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15:K20">
+    <cfRule type="containsBlanks" dxfId="2" priority="6">
+      <formula>LEN(TRIM(K15))=0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF4B317F"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15:K20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="4"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF331966"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
+      <formula>LEN(TRIM(K15))=0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF4B317F"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="1"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF4B317F"/>
+        <color rgb="FFAB7FFF"/>
+        <color rgb="FFF5F0FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
slowing down the decelerate portion
</commit_message>
<xml_diff>
--- a/animations/f_slow_stop.xlsx
+++ b/animations/f_slow_stop.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F710562A-9193-8C48-9D3B-0E0C7FDECC4D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{28896332-5CED-6D49-913A-D01441D13FAF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="50260" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,21 +127,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -475,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW81"/>
+  <dimension ref="A1:AW84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="266" zoomScaleNormal="266" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView tabSelected="1" zoomScale="266" zoomScaleNormal="266" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -600,178 +586,156 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4">
-        <v>7</v>
-      </c>
-      <c r="K4">
-        <v>8</v>
-      </c>
-    </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>1</v>
+      </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K5">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K6">
-        <v>7</v>
-      </c>
-      <c r="L6">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L7">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>1</v>
+      </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L8">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>1</v>
+      </c>
       <c r="H9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L9">
-        <v>6</v>
-      </c>
-      <c r="M9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>3</v>
-      </c>
-      <c r="L10">
-        <v>5</v>
-      </c>
-      <c r="M10">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
       <c r="K11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M11">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>1</v>
+      </c>
       <c r="K12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L12">
         <v>5</v>
@@ -781,8 +745,11 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <v>2</v>
+      </c>
       <c r="L13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M13">
         <v>8</v>
@@ -793,18 +760,15 @@
         <v>1</v>
       </c>
       <c r="L14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M14">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="K15">
-        <v>2</v>
-      </c>
       <c r="L15">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M15">
         <v>8</v>
@@ -812,10 +776,10 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="K16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M16">
         <v>8</v>
@@ -823,7 +787,7 @@
     </row>
     <row r="17" spans="9:13" x14ac:dyDescent="0.2">
       <c r="K17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L17">
         <v>8</v>
@@ -834,7 +798,7 @@
     </row>
     <row r="18" spans="9:13" x14ac:dyDescent="0.2">
       <c r="K18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L18">
         <v>8</v>
@@ -845,7 +809,7 @@
     </row>
     <row r="19" spans="9:13" x14ac:dyDescent="0.2">
       <c r="K19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L19">
         <v>8</v>
@@ -856,7 +820,7 @@
     </row>
     <row r="20" spans="9:13" x14ac:dyDescent="0.2">
       <c r="K20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L20">
         <v>8</v>
@@ -867,24 +831,24 @@
     </row>
     <row r="21" spans="9:13" x14ac:dyDescent="0.2">
       <c r="K21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L21">
         <v>8</v>
       </c>
       <c r="M21">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="9:13" x14ac:dyDescent="0.2">
       <c r="K22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L22">
         <v>8</v>
       </c>
       <c r="M22">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="9:13" x14ac:dyDescent="0.2">
@@ -895,7 +859,7 @@
         <v>8</v>
       </c>
       <c r="M23">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="9:13" x14ac:dyDescent="0.2">
@@ -906,7 +870,7 @@
         <v>8</v>
       </c>
       <c r="M24">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="9:13" x14ac:dyDescent="0.2">
@@ -917,13 +881,10 @@
         <v>8</v>
       </c>
       <c r="M25">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="9:13" x14ac:dyDescent="0.2">
-      <c r="J26" s="5">
-        <v>2</v>
-      </c>
       <c r="K26">
         <v>8</v>
       </c>
@@ -931,192 +892,183 @@
         <v>8</v>
       </c>
       <c r="M26">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="9:13" x14ac:dyDescent="0.2">
-      <c r="I27">
-        <v>2</v>
-      </c>
-      <c r="J27" s="6">
-        <v>3</v>
-      </c>
       <c r="K27">
         <v>8</v>
       </c>
       <c r="L27">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M27">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="9:13" x14ac:dyDescent="0.2">
-      <c r="I28">
-        <v>3</v>
-      </c>
-      <c r="J28" s="7">
-        <v>4</v>
+      <c r="J28" s="5">
+        <v>2</v>
       </c>
       <c r="K28">
         <v>8</v>
       </c>
       <c r="L28">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="M28">
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I29">
-        <v>4</v>
-      </c>
-      <c r="J29" s="8">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="J29" s="6">
+        <v>3</v>
       </c>
       <c r="K29">
         <v>8</v>
       </c>
       <c r="L29">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I30">
-        <v>5</v>
-      </c>
-      <c r="J30" s="9">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="J30" s="7">
+        <v>4</v>
       </c>
       <c r="K30">
         <v>8</v>
       </c>
       <c r="L30">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I31">
-        <v>6</v>
-      </c>
-      <c r="J31" s="10">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="J31" s="8">
+        <v>5</v>
       </c>
       <c r="K31">
         <v>8</v>
       </c>
       <c r="L31">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="9:13" x14ac:dyDescent="0.2">
       <c r="I32">
-        <v>7</v>
-      </c>
-      <c r="J32">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="J32" s="9">
+        <v>6</v>
       </c>
       <c r="K32">
         <v>8</v>
       </c>
       <c r="L32">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="H33">
-        <v>4</v>
-      </c>
       <c r="I33">
-        <v>8</v>
-      </c>
-      <c r="J33">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="J33" s="10">
+        <v>7</v>
       </c>
       <c r="K33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="H34">
-        <v>5</v>
-      </c>
       <c r="I34">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J34">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K34">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="L34">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="6:12" x14ac:dyDescent="0.2">
       <c r="H35">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I35">
         <v>8</v>
       </c>
       <c r="J35">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K35">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="6:12" x14ac:dyDescent="0.2">
       <c r="H36">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I36">
         <v>8</v>
       </c>
       <c r="J36">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K36">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="G37">
-        <v>4</v>
-      </c>
       <c r="H37">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I37">
         <v>8</v>
       </c>
       <c r="J37">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K37">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="G38">
-        <v>5</v>
-      </c>
       <c r="H38">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I38">
         <v>8</v>
       </c>
       <c r="J38">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K38">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G39">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H39">
         <v>8</v>
@@ -1125,15 +1077,15 @@
         <v>8</v>
       </c>
       <c r="J39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K39">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="6:12" x14ac:dyDescent="0.2">
       <c r="G40">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H40">
         <v>8</v>
@@ -1142,15 +1094,15 @@
         <v>8</v>
       </c>
       <c r="J40">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="F41">
-        <v>5</v>
-      </c>
       <c r="G41">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H41">
         <v>8</v>
@@ -1158,562 +1110,330 @@
       <c r="I41">
         <v>8</v>
       </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="F42">
-        <v>6</v>
-      </c>
       <c r="G42">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H42">
         <v>8</v>
       </c>
       <c r="I42">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F43">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G43">
         <v>8</v>
       </c>
       <c r="H43">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I43">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F44">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G44">
         <v>8</v>
       </c>
       <c r="H44">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I44">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F45">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G45">
         <v>8</v>
       </c>
       <c r="H45">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I45">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F46">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G46">
         <v>8</v>
       </c>
       <c r="H46">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I46">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F47">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G47">
         <v>8</v>
       </c>
       <c r="H47">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I47">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="6:12" x14ac:dyDescent="0.2">
       <c r="F48">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G48">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H48">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I48">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F49">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G49">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H49">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I49">
-        <v>8</v>
-      </c>
-      <c r="J49">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F50">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G50">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H50">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I50">
-        <v>7</v>
-      </c>
-      <c r="J50">
-        <v>8</v>
-      </c>
-      <c r="K50">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F51">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G51">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H51">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I51">
-        <v>6</v>
-      </c>
-      <c r="J51">
-        <v>8</v>
-      </c>
-      <c r="K51">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F52">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G52">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H52">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I52">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J52">
         <v>8</v>
       </c>
-      <c r="K52">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>3</v>
+      </c>
       <c r="G53">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H53">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I53">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J53">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K53">
         <v>8</v>
       </c>
-      <c r="L53">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>2</v>
+      </c>
       <c r="G54">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H54">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I54">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J54">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K54">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L54">
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="M54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
       <c r="H55">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I55">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J55">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K55">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L55">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="H56">
-        <v>2</v>
-      </c>
-      <c r="I56">
-        <v>2</v>
-      </c>
-      <c r="J56">
-        <v>4</v>
-      </c>
-      <c r="K56">
-        <v>7</v>
-      </c>
-      <c r="L56">
-        <v>8</v>
-      </c>
-      <c r="M56">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A57" s="4"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="10"/>
-      <c r="H57">
-        <v>1</v>
-      </c>
-      <c r="I57">
-        <v>2</v>
-      </c>
-      <c r="J57">
-        <v>3</v>
-      </c>
-      <c r="K57">
-        <v>6</v>
-      </c>
-      <c r="L57">
-        <v>8</v>
-      </c>
-      <c r="M57">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I58">
-        <v>2</v>
-      </c>
-      <c r="J58">
-        <v>2</v>
-      </c>
-      <c r="K58">
-        <v>5</v>
-      </c>
-      <c r="L58">
-        <v>7</v>
-      </c>
-      <c r="M58">
-        <v>8</v>
-      </c>
-      <c r="N58">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I59">
-        <v>1</v>
-      </c>
-      <c r="J59">
-        <v>2</v>
-      </c>
-      <c r="K59">
-        <v>4</v>
-      </c>
-      <c r="L59">
-        <v>6</v>
-      </c>
-      <c r="M59">
-        <v>7</v>
-      </c>
-      <c r="N59">
-        <v>8</v>
-      </c>
-      <c r="O59">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I60">
-        <v>1</v>
-      </c>
-      <c r="J60">
-        <v>2</v>
-      </c>
-      <c r="K60">
-        <v>3</v>
-      </c>
-      <c r="L60">
-        <v>5</v>
-      </c>
-      <c r="M60">
-        <v>6</v>
-      </c>
-      <c r="N60">
-        <v>7</v>
-      </c>
-      <c r="O60">
-        <v>8</v>
-      </c>
-      <c r="P60">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I61">
-        <v>1</v>
-      </c>
-      <c r="J61">
-        <v>2</v>
-      </c>
-      <c r="K61">
-        <v>3</v>
-      </c>
-      <c r="L61">
-        <v>4</v>
-      </c>
-      <c r="M61">
-        <v>5</v>
-      </c>
-      <c r="N61">
-        <v>6</v>
-      </c>
-      <c r="O61">
-        <v>7</v>
-      </c>
-      <c r="P61">
-        <v>8</v>
-      </c>
-      <c r="Q61">
-        <v>8</v>
-      </c>
-      <c r="U61"/>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I62">
-        <v>1</v>
-      </c>
-      <c r="J62">
-        <v>2</v>
-      </c>
-      <c r="K62">
-        <v>3</v>
-      </c>
-      <c r="L62">
-        <v>5</v>
-      </c>
-      <c r="M62">
-        <v>6</v>
-      </c>
-      <c r="N62">
-        <v>7</v>
-      </c>
-      <c r="O62">
-        <v>8</v>
-      </c>
-      <c r="P62">
-        <v>8</v>
-      </c>
-      <c r="U62"/>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I63">
-        <v>1</v>
-      </c>
-      <c r="J63">
-        <v>2</v>
-      </c>
-      <c r="K63">
-        <v>3</v>
-      </c>
-      <c r="L63">
-        <v>4</v>
-      </c>
-      <c r="M63">
-        <v>5</v>
-      </c>
-      <c r="N63">
-        <v>6</v>
-      </c>
-      <c r="O63">
-        <v>7</v>
-      </c>
-      <c r="P63">
-        <v>8</v>
-      </c>
-      <c r="Q63">
-        <v>8</v>
-      </c>
-      <c r="U63"/>
-    </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="I64">
-        <v>1</v>
-      </c>
-      <c r="J64">
-        <v>2</v>
-      </c>
-      <c r="K64">
-        <v>3</v>
-      </c>
-      <c r="L64">
-        <v>5</v>
-      </c>
-      <c r="M64">
-        <v>6</v>
-      </c>
-      <c r="N64">
-        <v>7</v>
-      </c>
-      <c r="O64">
-        <v>8</v>
-      </c>
-      <c r="P64">
-        <v>8</v>
-      </c>
-      <c r="V64" s="1"/>
-      <c r="W64" s="1"/>
-      <c r="X64" s="1"/>
-    </row>
-    <row r="65" spans="9:49" x14ac:dyDescent="0.2">
-      <c r="I65">
-        <v>1</v>
-      </c>
-      <c r="J65">
-        <v>2</v>
-      </c>
-      <c r="K65">
-        <v>3</v>
-      </c>
-      <c r="L65">
-        <v>4</v>
-      </c>
-      <c r="M65">
-        <v>5</v>
-      </c>
-      <c r="N65">
-        <v>6</v>
-      </c>
-      <c r="O65">
-        <v>7</v>
-      </c>
-      <c r="P65">
-        <v>8</v>
-      </c>
-      <c r="Q65">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="9:49" x14ac:dyDescent="0.2">
-      <c r="AV68" s="2"/>
-    </row>
-    <row r="69" spans="9:49" x14ac:dyDescent="0.2">
-      <c r="AO69" s="2"/>
-      <c r="AP69" s="3"/>
-      <c r="AV69" s="2"/>
-      <c r="AW69" s="3"/>
-    </row>
-    <row r="70" spans="9:49" x14ac:dyDescent="0.2">
-      <c r="AO70" s="2"/>
-      <c r="AP70" s="3"/>
-      <c r="AV70" s="2"/>
-      <c r="AW70" s="3"/>
-    </row>
-    <row r="71" spans="9:49" x14ac:dyDescent="0.2">
-      <c r="AO71" s="2"/>
-      <c r="AP71" s="3"/>
-      <c r="AU71" s="2"/>
-      <c r="AV71" s="3"/>
-    </row>
-    <row r="72" spans="9:49" x14ac:dyDescent="0.2">
-      <c r="AO72" s="3"/>
-      <c r="AP72" s="2"/>
-      <c r="AU72" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="M55">
+        <v>8</v>
+      </c>
+      <c r="N55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A60" s="4"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="10"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U64"/>
+    </row>
+    <row r="65" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="U65"/>
+    </row>
+    <row r="66" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="U66"/>
+    </row>
+    <row r="67" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+    </row>
+    <row r="71" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="AV71" s="2"/>
+    </row>
+    <row r="72" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="AO72" s="2"/>
+      <c r="AP72" s="3"/>
       <c r="AV72" s="2"/>
-    </row>
-    <row r="73" spans="9:49" x14ac:dyDescent="0.2">
-      <c r="AO73" s="3"/>
-      <c r="AP73" s="2"/>
-      <c r="AU73" s="3"/>
-    </row>
-    <row r="74" spans="9:49" x14ac:dyDescent="0.2">
-      <c r="AO74" s="3"/>
-      <c r="AP74" s="2"/>
-    </row>
-    <row r="75" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AW72" s="3"/>
+    </row>
+    <row r="73" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="AO73" s="2"/>
+      <c r="AP73" s="3"/>
+      <c r="AV73" s="2"/>
+      <c r="AW73" s="3"/>
+    </row>
+    <row r="74" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="AO74" s="2"/>
+      <c r="AP74" s="3"/>
+      <c r="AU74" s="2"/>
+      <c r="AV74" s="3"/>
+    </row>
+    <row r="75" spans="21:49" x14ac:dyDescent="0.2">
       <c r="AO75" s="3"/>
       <c r="AP75" s="2"/>
-    </row>
-    <row r="76" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AU75" s="3"/>
+      <c r="AV75" s="2"/>
+    </row>
+    <row r="76" spans="21:49" x14ac:dyDescent="0.2">
       <c r="AO76" s="3"/>
       <c r="AP76" s="2"/>
-    </row>
-    <row r="77" spans="9:49" x14ac:dyDescent="0.2">
+      <c r="AU76" s="3"/>
+    </row>
+    <row r="77" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="AO77" s="3"/>
       <c r="AP77" s="2"/>
     </row>
-    <row r="78" spans="9:49" x14ac:dyDescent="0.2">
+    <row r="78" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="AO78" s="3"/>
       <c r="AP78" s="2"/>
     </row>
-    <row r="79" spans="9:49" x14ac:dyDescent="0.2">
+    <row r="79" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="AO79" s="3"/>
       <c r="AP79" s="2"/>
     </row>
-    <row r="80" spans="9:49" x14ac:dyDescent="0.2">
+    <row r="80" spans="21:49" x14ac:dyDescent="0.2">
       <c r="AP80" s="2"/>
     </row>
     <row r="81" spans="42:42" x14ac:dyDescent="0.2">
       <c r="AP81" s="2"/>
     </row>
+    <row r="82" spans="42:42" x14ac:dyDescent="0.2">
+      <c r="AP82" s="2"/>
+    </row>
+    <row r="83" spans="42:42" x14ac:dyDescent="0.2">
+      <c r="AP83" s="2"/>
+    </row>
+    <row r="84" spans="42:42" x14ac:dyDescent="0.2">
+      <c r="AP84" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="AI66:AT66 AW71:BT118 AS66:XFD75 A71:AQ75 A66:AP70 AV67:AW76 AK67:BD67 AV71:BI96 AR67:BI75 AY67:BD81 AN68:AP76 AO68:AV68 A76:XFD1048576 AQ68:BH75 AU71:BH94 AT74:BB94 AQ68:BC81 AS75:BB94 J57:XFD58 A58:N58 I58:Q59 A59:XFD65 H49:Q57 A26:I31 K26:XFD31 A21:XFD25 A14:J20 L14:XFD20 A1:XFD13 A32:XFD56 J49:Q63">
-    <cfRule type="containsBlanks" dxfId="8" priority="18">
+  <conditionalFormatting sqref="AI69:AT69 AW74:BT121 AS69:XFD78 A74:AQ78 A69:AP73 AV70:AW79 AK70:BD70 AV74:BI99 AR70:BI78 AY70:BD84 AN71:AP79 AO71:AV71 A79:XFD1048576 AQ71:BH78 AU74:BH97 AT77:BB97 AQ71:BC84 AS78:BB97 J60:XFD61 H52:Q60 A28:I33 K28:XFD33 A23:XFD27 A16:J22 L16:XFD22 A1:XFD15 J52:Q66 A61:P61 I61:S62 L54:S64 J54:S60 F54:I64 A62:XFD68 A34:XFD59">
+    <cfRule type="containsBlanks" dxfId="6" priority="18">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="19">
@@ -1727,7 +1447,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J57:XFD58 A58:N58 I58:Q59 A59:XFD1048576 H49:Q57 A26:I31 K26:XFD31 A21:XFD25 A14:J20 L14:XFD20 A1:XFD13 A32:XFD56 J49:Q63">
+  <conditionalFormatting sqref="J60:XFD61 H52:Q60 A28:I33 K28:XFD33 A23:XFD27 A16:J22 L16:XFD22 A1:XFD15 J52:Q66 A61:P61 I61:S62 L54:S64 J54:S60 F54:I64 A62:XFD1048576 A34:XFD59">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -1738,7 +1458,7 @@
         <color rgb="FFF5F0FF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="7" priority="15">
+    <cfRule type="containsBlanks" dxfId="5" priority="15">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="16">
@@ -1762,9 +1482,9 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K14">
+  <conditionalFormatting sqref="K16">
     <cfRule type="containsBlanks" dxfId="4" priority="12">
-      <formula>LEN(TRIM(K14))=0</formula>
+      <formula>LEN(TRIM(K16))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="13">
       <colorScale>
@@ -1777,7 +1497,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K14">
+  <conditionalFormatting sqref="K16">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -1789,7 +1509,7 @@
       </colorScale>
     </cfRule>
     <cfRule type="containsBlanks" dxfId="3" priority="9">
-      <formula>LEN(TRIM(K14))=0</formula>
+      <formula>LEN(TRIM(K16))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
       <colorScale>
@@ -1812,9 +1532,9 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K15:K20">
+  <conditionalFormatting sqref="K17:K22">
     <cfRule type="containsBlanks" dxfId="2" priority="6">
-      <formula>LEN(TRIM(K15))=0</formula>
+      <formula>LEN(TRIM(K17))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="7">
       <colorScale>
@@ -1827,7 +1547,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K15:K20">
+  <conditionalFormatting sqref="K17:K22">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -1839,7 +1559,7 @@
       </colorScale>
     </cfRule>
     <cfRule type="containsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(K15))=0</formula>
+      <formula>LEN(TRIM(K17))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
       <colorScale>

</xml_diff>

<commit_message>
minor adjustments to slow stop
</commit_message>
<xml_diff>
--- a/animations/f_slow_stop.xlsx
+++ b/animations/f_slow_stop.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{28896332-5CED-6D49-913A-D01441D13FAF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADE811B-E517-471A-BA9A-4D81FC1C1000}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="50260" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="50265" windowHeight="28335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -461,20 +465,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW84"/>
+  <dimension ref="A1:AW85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="266" zoomScaleNormal="266" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="20" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="66" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="15" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="66" width="2.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -526,9 +532,26 @@
       <c r="Q1">
         <v>7</v>
       </c>
-      <c r="U1"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R1">
+        <v>8</v>
+      </c>
+      <c r="S1">
+        <v>9</v>
+      </c>
+      <c r="T1">
+        <v>0</v>
+      </c>
+      <c r="U1">
+        <v>1</v>
+      </c>
+      <c r="V1">
+        <v>2</v>
+      </c>
+      <c r="W1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -557,7 +580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -586,79 +609,99 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C5">
-        <v>1</v>
-      </c>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="D6">
-        <v>1</v>
-      </c>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="E7">
-        <v>1</v>
-      </c>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K7">
         <v>7</v>
@@ -667,21 +710,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="F8">
-        <v>1</v>
-      </c>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K8">
         <v>6</v>
@@ -690,115 +730,117 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K9">
         <v>5</v>
       </c>
       <c r="L9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="J12">
-        <v>1</v>
-      </c>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M13">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="K14">
-        <v>1</v>
-      </c>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M14">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M15">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="K16">
-        <v>1</v>
-      </c>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M16">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M17">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L18">
         <v>8</v>
@@ -807,9 +849,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L19">
         <v>8</v>
@@ -818,9 +860,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L20">
         <v>8</v>
@@ -829,9 +871,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L21">
         <v>8</v>
@@ -840,9 +882,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L22">
         <v>8</v>
@@ -851,18 +893,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L23">
         <v>8</v>
       </c>
       <c r="M23">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="9:13" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K24">
         <v>8</v>
       </c>
@@ -870,10 +912,10 @@
         <v>8</v>
       </c>
       <c r="M24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="9:13" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K25">
         <v>8</v>
       </c>
@@ -881,10 +923,10 @@
         <v>8</v>
       </c>
       <c r="M25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="9:13" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K26">
         <v>8</v>
       </c>
@@ -892,10 +934,10 @@
         <v>8</v>
       </c>
       <c r="M26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="9:13" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K27">
         <v>8</v>
       </c>
@@ -903,13 +945,10 @@
         <v>8</v>
       </c>
       <c r="M27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="9:13" x14ac:dyDescent="0.2">
-      <c r="J28" s="5">
-        <v>2</v>
-      </c>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="9:13" x14ac:dyDescent="0.25">
       <c r="K28">
         <v>8</v>
       </c>
@@ -917,175 +956,172 @@
         <v>8</v>
       </c>
       <c r="M28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="9:13" x14ac:dyDescent="0.2">
-      <c r="I29">
-        <v>2</v>
-      </c>
-      <c r="J29" s="6">
-        <v>3</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J29" s="5">
+        <v>2</v>
       </c>
       <c r="K29">
         <v>8</v>
       </c>
       <c r="L29">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="9:13" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I30">
-        <v>3</v>
-      </c>
-      <c r="J30" s="7">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="J30" s="6">
+        <v>3</v>
       </c>
       <c r="K30">
         <v>8</v>
       </c>
       <c r="L30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="9:13" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I31">
-        <v>4</v>
-      </c>
-      <c r="J31" s="8">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="J31" s="7">
+        <v>4</v>
       </c>
       <c r="K31">
         <v>8</v>
       </c>
       <c r="L31">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="9:13" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I32">
-        <v>5</v>
-      </c>
-      <c r="J32" s="9">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="J32" s="8">
+        <v>5</v>
       </c>
       <c r="K32">
         <v>8</v>
       </c>
       <c r="L32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="6:12" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="6:12" x14ac:dyDescent="0.25">
       <c r="I33">
-        <v>6</v>
-      </c>
-      <c r="J33" s="10">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="J33" s="9">
+        <v>6</v>
       </c>
       <c r="K33">
         <v>8</v>
       </c>
       <c r="L33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="6:12" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="6:12" x14ac:dyDescent="0.25">
       <c r="I34">
-        <v>7</v>
-      </c>
-      <c r="J34">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="J34" s="10">
+        <v>7</v>
       </c>
       <c r="K34">
         <v>8</v>
       </c>
       <c r="L34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="H35">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="6:12" x14ac:dyDescent="0.25">
       <c r="I35">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J35">
         <v>8</v>
       </c>
       <c r="K35">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="6:12" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I36">
         <v>8</v>
       </c>
       <c r="J36">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="6:12" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I37">
         <v>8</v>
       </c>
       <c r="J37">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="6:12" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H38">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I38">
         <v>8</v>
       </c>
       <c r="J38">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="G39">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="6:12" x14ac:dyDescent="0.25">
       <c r="H39">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I39">
         <v>8</v>
       </c>
       <c r="J39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="6:12" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="6:12" x14ac:dyDescent="0.25">
       <c r="G40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H40">
         <v>8</v>
@@ -1094,15 +1130,15 @@
         <v>8</v>
       </c>
       <c r="J40">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="6:12" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="6:12" x14ac:dyDescent="0.25">
       <c r="G41">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H41">
         <v>8</v>
@@ -1111,15 +1147,15 @@
         <v>8</v>
       </c>
       <c r="J41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="6:12" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="6:12" x14ac:dyDescent="0.25">
       <c r="G42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H42">
         <v>8</v>
@@ -1128,15 +1164,15 @@
         <v>8</v>
       </c>
       <c r="J42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="F43">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="6:12" x14ac:dyDescent="0.25">
       <c r="G43">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H43">
         <v>8</v>
@@ -1144,10 +1180,13 @@
       <c r="I43">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="6:12" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G44">
         <v>8</v>
@@ -1156,38 +1195,38 @@
         <v>8</v>
       </c>
       <c r="I44">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="6:12" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F45">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G45">
         <v>8</v>
       </c>
       <c r="H45">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I45">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="6:12" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G46">
         <v>8</v>
       </c>
       <c r="H46">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I46">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="6:12" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F47">
         <v>8</v>
       </c>
@@ -1195,13 +1234,13 @@
         <v>8</v>
       </c>
       <c r="H47">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="6:12" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F48">
         <v>8</v>
       </c>
@@ -1209,29 +1248,29 @@
         <v>8</v>
       </c>
       <c r="H48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F49">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G49">
         <v>8</v>
       </c>
       <c r="H49">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G50">
         <v>8</v>
@@ -1240,199 +1279,437 @@
         <v>8</v>
       </c>
       <c r="I50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F51">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G51">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H51">
         <v>8</v>
       </c>
       <c r="I51">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G52">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H52">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I52">
         <v>8</v>
       </c>
-      <c r="J52">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G53">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H53">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I53">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J53">
         <v>8</v>
       </c>
-      <c r="K53">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F54">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G54">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H54">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I54">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J54">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K54">
-        <v>7</v>
-      </c>
-      <c r="L54">
-        <v>8</v>
-      </c>
-      <c r="M54">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G55">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H55">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I55">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J55">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K55">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L55">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M55">
         <v>8</v>
       </c>
-      <c r="N55">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A60" s="4"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="10"/>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="U64"/>
-    </row>
-    <row r="65" spans="21:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>4</v>
+      </c>
+      <c r="I56">
+        <v>5</v>
+      </c>
+      <c r="J56">
+        <v>6</v>
+      </c>
+      <c r="K56">
+        <v>6</v>
+      </c>
+      <c r="L56">
+        <v>7</v>
+      </c>
+      <c r="M56">
+        <v>7</v>
+      </c>
+      <c r="N56">
+        <v>8</v>
+      </c>
+      <c r="O56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+      <c r="H57">
+        <v>3</v>
+      </c>
+      <c r="I57">
+        <v>4</v>
+      </c>
+      <c r="J57">
+        <v>5</v>
+      </c>
+      <c r="K57">
+        <v>5</v>
+      </c>
+      <c r="L57">
+        <v>6</v>
+      </c>
+      <c r="M57">
+        <v>6</v>
+      </c>
+      <c r="N57">
+        <v>7</v>
+      </c>
+      <c r="O57">
+        <v>7</v>
+      </c>
+      <c r="P57">
+        <v>8</v>
+      </c>
+      <c r="Q57">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58">
+        <v>3</v>
+      </c>
+      <c r="J58">
+        <v>4</v>
+      </c>
+      <c r="K58">
+        <v>4</v>
+      </c>
+      <c r="L58">
+        <v>5</v>
+      </c>
+      <c r="M58">
+        <v>5</v>
+      </c>
+      <c r="N58">
+        <v>6</v>
+      </c>
+      <c r="O58">
+        <v>6</v>
+      </c>
+      <c r="P58">
+        <v>7</v>
+      </c>
+      <c r="Q58">
+        <v>8</v>
+      </c>
+      <c r="R58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>2</v>
+      </c>
+      <c r="J59">
+        <v>3</v>
+      </c>
+      <c r="K59">
+        <v>3</v>
+      </c>
+      <c r="L59">
+        <v>4</v>
+      </c>
+      <c r="M59">
+        <v>4</v>
+      </c>
+      <c r="N59">
+        <v>5</v>
+      </c>
+      <c r="O59">
+        <v>5</v>
+      </c>
+      <c r="P59">
+        <v>6</v>
+      </c>
+      <c r="Q59">
+        <v>7</v>
+      </c>
+      <c r="R59">
+        <v>7</v>
+      </c>
+      <c r="S59">
+        <v>8</v>
+      </c>
+      <c r="T59">
+        <v>8</v>
+      </c>
+      <c r="U59"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>2</v>
+      </c>
+      <c r="K60">
+        <v>2</v>
+      </c>
+      <c r="L60">
+        <v>3</v>
+      </c>
+      <c r="M60">
+        <v>3</v>
+      </c>
+      <c r="N60">
+        <v>4</v>
+      </c>
+      <c r="O60">
+        <v>4</v>
+      </c>
+      <c r="P60">
+        <v>5</v>
+      </c>
+      <c r="Q60">
+        <v>6</v>
+      </c>
+      <c r="R60">
+        <v>6</v>
+      </c>
+      <c r="S60">
+        <v>7</v>
+      </c>
+      <c r="T60">
+        <v>8</v>
+      </c>
+      <c r="U60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="10"/>
+      <c r="L61">
+        <v>1</v>
+      </c>
+      <c r="M61">
+        <v>2</v>
+      </c>
+      <c r="N61">
+        <v>3</v>
+      </c>
+      <c r="O61">
+        <v>3</v>
+      </c>
+      <c r="P61">
+        <v>4</v>
+      </c>
+      <c r="Q61">
+        <v>4</v>
+      </c>
+      <c r="R61">
+        <v>5</v>
+      </c>
+      <c r="S61">
+        <v>6</v>
+      </c>
+      <c r="T61">
+        <v>7</v>
+      </c>
+      <c r="U61" s="1">
+        <v>8</v>
+      </c>
+      <c r="V61">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="O62">
+        <v>1</v>
+      </c>
+      <c r="P62">
+        <v>2</v>
+      </c>
+      <c r="Q62">
+        <v>3</v>
+      </c>
+      <c r="R62">
+        <v>4</v>
+      </c>
+      <c r="S62">
+        <v>5</v>
+      </c>
+      <c r="T62">
+        <v>6</v>
+      </c>
+      <c r="U62" s="1">
+        <v>7</v>
+      </c>
+      <c r="V62">
+        <v>8</v>
+      </c>
+      <c r="W62">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="21:49" x14ac:dyDescent="0.25">
       <c r="U65"/>
     </row>
-    <row r="66" spans="21:49" x14ac:dyDescent="0.2">
+    <row r="66" spans="21:49" x14ac:dyDescent="0.25">
       <c r="U66"/>
     </row>
-    <row r="67" spans="21:49" x14ac:dyDescent="0.2">
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
-      <c r="X67" s="1"/>
-    </row>
-    <row r="71" spans="21:49" x14ac:dyDescent="0.2">
-      <c r="AV71" s="2"/>
-    </row>
-    <row r="72" spans="21:49" x14ac:dyDescent="0.2">
-      <c r="AO72" s="2"/>
-      <c r="AP72" s="3"/>
+    <row r="67" spans="21:49" x14ac:dyDescent="0.25">
+      <c r="U67"/>
+    </row>
+    <row r="68" spans="21:49" x14ac:dyDescent="0.25">
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+    </row>
+    <row r="72" spans="21:49" x14ac:dyDescent="0.25">
       <c r="AV72" s="2"/>
-      <c r="AW72" s="3"/>
-    </row>
-    <row r="73" spans="21:49" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="21:49" x14ac:dyDescent="0.25">
       <c r="AO73" s="2"/>
       <c r="AP73" s="3"/>
       <c r="AV73" s="2"/>
       <c r="AW73" s="3"/>
     </row>
-    <row r="74" spans="21:49" x14ac:dyDescent="0.2">
+    <row r="74" spans="21:49" x14ac:dyDescent="0.25">
       <c r="AO74" s="2"/>
       <c r="AP74" s="3"/>
-      <c r="AU74" s="2"/>
-      <c r="AV74" s="3"/>
-    </row>
-    <row r="75" spans="21:49" x14ac:dyDescent="0.2">
-      <c r="AO75" s="3"/>
-      <c r="AP75" s="2"/>
-      <c r="AU75" s="3"/>
-      <c r="AV75" s="2"/>
-    </row>
-    <row r="76" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="AV74" s="2"/>
+      <c r="AW74" s="3"/>
+    </row>
+    <row r="75" spans="21:49" x14ac:dyDescent="0.25">
+      <c r="AO75" s="2"/>
+      <c r="AP75" s="3"/>
+      <c r="AU75" s="2"/>
+      <c r="AV75" s="3"/>
+    </row>
+    <row r="76" spans="21:49" x14ac:dyDescent="0.25">
       <c r="AO76" s="3"/>
       <c r="AP76" s="2"/>
       <c r="AU76" s="3"/>
-    </row>
-    <row r="77" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="AV76" s="2"/>
+    </row>
+    <row r="77" spans="21:49" x14ac:dyDescent="0.25">
       <c r="AO77" s="3"/>
       <c r="AP77" s="2"/>
-    </row>
-    <row r="78" spans="21:49" x14ac:dyDescent="0.2">
+      <c r="AU77" s="3"/>
+    </row>
+    <row r="78" spans="21:49" x14ac:dyDescent="0.25">
       <c r="AO78" s="3"/>
       <c r="AP78" s="2"/>
     </row>
-    <row r="79" spans="21:49" x14ac:dyDescent="0.2">
+    <row r="79" spans="21:49" x14ac:dyDescent="0.25">
       <c r="AO79" s="3"/>
       <c r="AP79" s="2"/>
     </row>
-    <row r="80" spans="21:49" x14ac:dyDescent="0.2">
+    <row r="80" spans="21:49" x14ac:dyDescent="0.25">
+      <c r="AO80" s="3"/>
       <c r="AP80" s="2"/>
     </row>
-    <row r="81" spans="42:42" x14ac:dyDescent="0.2">
+    <row r="81" spans="42:42" x14ac:dyDescent="0.25">
       <c r="AP81" s="2"/>
     </row>
-    <row r="82" spans="42:42" x14ac:dyDescent="0.2">
+    <row r="82" spans="42:42" x14ac:dyDescent="0.25">
       <c r="AP82" s="2"/>
     </row>
-    <row r="83" spans="42:42" x14ac:dyDescent="0.2">
+    <row r="83" spans="42:42" x14ac:dyDescent="0.25">
       <c r="AP83" s="2"/>
     </row>
-    <row r="84" spans="42:42" x14ac:dyDescent="0.2">
+    <row r="84" spans="42:42" x14ac:dyDescent="0.25">
       <c r="AP84" s="2"/>
     </row>
+    <row r="85" spans="42:42" x14ac:dyDescent="0.25">
+      <c r="AP85" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="AI69:AT69 AW74:BT121 AS69:XFD78 A74:AQ78 A69:AP73 AV70:AW79 AK70:BD70 AV74:BI99 AR70:BI78 AY70:BD84 AN71:AP79 AO71:AV71 A79:XFD1048576 AQ71:BH78 AU74:BH97 AT77:BB97 AQ71:BC84 AS78:BB97 J60:XFD61 H52:Q60 A28:I33 K28:XFD33 A23:XFD27 A16:J22 L16:XFD22 A1:XFD15 J52:Q66 A61:P61 I61:S62 L54:S64 J54:S60 F54:I64 A62:XFD68 A34:XFD59">
+  <conditionalFormatting sqref="AI70:AT70 AW75:BT122 AS70:XFD79 A75:AQ79 A70:AP74 AV71:AW80 AK71:BD71 AV75:BI100 AR71:BI79 AY71:BD85 AN72:AP80 AO72:AV72 A80:XFD1048576 AQ72:BH79 AU75:BH98 AT78:BB98 AQ72:BC85 AS79:BB98 J61:XFD62 H53:Q61 A29:I34 K29:XFD34 A24:XFD28 A17:J23 L17:XFD23 J53:Q67 A62:P62 I62:S63 L55:S65 J55:S61 F55:I65 A63:XFD69 A1:XFD16 A35:XFD60">
     <cfRule type="containsBlanks" dxfId="6" priority="18">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
@@ -1447,7 +1724,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J60:XFD61 H52:Q60 A28:I33 K28:XFD33 A23:XFD27 A16:J22 L16:XFD22 A1:XFD15 J52:Q66 A61:P61 I61:S62 L54:S64 J54:S60 F54:I64 A62:XFD1048576 A34:XFD59">
+  <conditionalFormatting sqref="J61:XFD62 H53:Q61 A29:I34 K29:XFD34 A24:XFD28 A17:J23 L17:XFD23 J53:Q67 A62:P62 I62:S63 L55:S65 J55:S61 F55:I65 A63:XFD1048576 A1:XFD16 A35:XFD60">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -1482,9 +1759,9 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
+  <conditionalFormatting sqref="K17">
     <cfRule type="containsBlanks" dxfId="4" priority="12">
-      <formula>LEN(TRIM(K16))=0</formula>
+      <formula>LEN(TRIM(K17))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="13">
       <colorScale>
@@ -1497,7 +1774,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
+  <conditionalFormatting sqref="K17">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -1509,7 +1786,7 @@
       </colorScale>
     </cfRule>
     <cfRule type="containsBlanks" dxfId="3" priority="9">
-      <formula>LEN(TRIM(K16))=0</formula>
+      <formula>LEN(TRIM(K17))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
       <colorScale>
@@ -1532,9 +1809,9 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17:K22">
+  <conditionalFormatting sqref="K18:K23">
     <cfRule type="containsBlanks" dxfId="2" priority="6">
-      <formula>LEN(TRIM(K17))=0</formula>
+      <formula>LEN(TRIM(K18))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="7">
       <colorScale>
@@ -1547,7 +1824,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17:K22">
+  <conditionalFormatting sqref="K18:K23">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -1559,7 +1836,7 @@
       </colorScale>
     </cfRule>
     <cfRule type="containsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(K17))=0</formula>
+      <formula>LEN(TRIM(K18))=0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
       <colorScale>

</xml_diff>